<commit_message>
changes to dataset to be publication ready.
</commit_message>
<xml_diff>
--- a/data_ophonus_a2_c.xlsx
+++ b/data_ophonus_a2_c.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mendelu-my.sharepoint.com/personal/xstoces_mendelu_cz1/Documents/SSD_21.12.2024/Maďarsko/excel/Ophonus/a2/new/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Deeplearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="11_AD4D80C4656A4B7AC02E7484B35F43565BDEDD8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E2176D0-F6EE-4887-8560-C8E00BA2AAC6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688FE479-3E98-42C2-BFCA-9A759920F86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27735" yWindow="1875" windowWidth="21570" windowHeight="18105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26325" yWindow="0" windowWidth="24000" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,6 +240,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -255,10 +256,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,10 +524,13 @@
   <dimension ref="A1:T215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -691,7 +691,7 @@
       <c r="L3">
         <v>2</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="5">
         <v>0.23385397599999999</v>
       </c>
       <c r="N3" s="2">
@@ -750,7 +750,7 @@
       <c r="L4">
         <v>3</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="5">
         <v>0.21167241000000001</v>
       </c>
       <c r="N4" s="2">
@@ -809,7 +809,7 @@
       <c r="L5">
         <v>3</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="5">
         <v>0.2121860216</v>
       </c>
       <c r="N5" s="2">
@@ -868,7 +868,7 @@
       <c r="L6">
         <v>3</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="5">
         <v>0.21951849500000001</v>
       </c>
       <c r="N6" s="2">
@@ -1757,7 +1757,7 @@
       <c r="L21">
         <v>3</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="5">
         <v>0.20198213700000001</v>
       </c>
       <c r="N21" s="2">
@@ -1816,7 +1816,7 @@
       <c r="L22">
         <v>2</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="5">
         <v>0.231511311</v>
       </c>
       <c r="N22" s="2">
@@ -1875,7 +1875,7 @@
       <c r="L23">
         <v>2</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="5">
         <v>0.231511311</v>
       </c>
       <c r="N23" s="2">
@@ -1934,7 +1934,7 @@
       <c r="L24">
         <v>3</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="5">
         <v>0.21742198099999999</v>
       </c>
       <c r="N24" s="2">
@@ -1993,7 +1993,7 @@
       <c r="L25">
         <v>3</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="5">
         <v>0.237421981</v>
       </c>
       <c r="N25" s="2">
@@ -2052,7 +2052,7 @@
       <c r="L26">
         <v>3</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="5">
         <v>0.21932320699999999</v>
       </c>
       <c r="N26" s="2">
@@ -2111,7 +2111,7 @@
       <c r="L27">
         <v>3</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="5">
         <v>0.21932320699999999</v>
       </c>
       <c r="N27" s="2">
@@ -2170,7 +2170,7 @@
       <c r="L28">
         <v>2</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="5">
         <v>0.22828552999999999</v>
       </c>
       <c r="N28" s="2">
@@ -2229,7 +2229,7 @@
       <c r="L29">
         <v>2</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="5">
         <v>0.22828552999999999</v>
       </c>
       <c r="N29" s="2">
@@ -2288,7 +2288,7 @@
       <c r="L30">
         <v>3</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="5">
         <v>0.20318757700000001</v>
       </c>
       <c r="N30" s="2">
@@ -2347,7 +2347,7 @@
       <c r="L31">
         <v>3</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="5">
         <v>0.20318757700000001</v>
       </c>
       <c r="N31" s="2">
@@ -7539,7 +7539,7 @@
       <c r="L119">
         <v>3</v>
       </c>
-      <c r="M119" s="2">
+      <c r="M119" s="5">
         <v>0.19098489799999999</v>
       </c>
       <c r="N119" s="2">
@@ -7598,7 +7598,7 @@
       <c r="L120">
         <v>3</v>
       </c>
-      <c r="M120" s="2">
+      <c r="M120" s="5">
         <v>0.21630492500000001</v>
       </c>
       <c r="N120" s="2">
@@ -7657,7 +7657,7 @@
       <c r="L121">
         <v>3</v>
       </c>
-      <c r="M121" s="2">
+      <c r="M121" s="5">
         <v>0.21630492500000001</v>
       </c>
       <c r="N121" s="2">
@@ -7716,7 +7716,7 @@
       <c r="L122">
         <v>3</v>
       </c>
-      <c r="M122" s="4">
+      <c r="M122" s="5">
         <v>0.19802451500000001</v>
       </c>
       <c r="N122" s="2">
@@ -7775,7 +7775,7 @@
       <c r="L123">
         <v>3</v>
       </c>
-      <c r="M123" s="4">
+      <c r="M123" s="5">
         <v>0.19802451500000001</v>
       </c>
       <c r="N123" s="2">
@@ -7834,7 +7834,7 @@
       <c r="L124">
         <v>3</v>
       </c>
-      <c r="M124" s="2">
+      <c r="M124" s="5">
         <v>0.24276869400000001</v>
       </c>
       <c r="N124" s="2">
@@ -8247,20 +8247,20 @@
       <c r="L131" s="3">
         <v>3</v>
       </c>
-      <c r="M131" s="2">
+      <c r="M131" s="4">
         <v>0.22111041000000001</v>
       </c>
-      <c r="N131" s="2">
+      <c r="N131" s="4">
         <v>0.22190491800000001</v>
       </c>
-      <c r="O131" s="2">
+      <c r="O131" s="4">
         <v>4.1057874630000004</v>
       </c>
-      <c r="P131">
+      <c r="P131" s="3">
         <f t="shared" si="8"/>
         <v>3.5868194610187364E-3</v>
       </c>
-      <c r="Q131">
+      <c r="Q131" s="3">
         <f>ABS(N131-M131)/$T$14</f>
         <v>3.7160263287242751E-3</v>
       </c>
@@ -10080,20 +10080,20 @@
       <c r="L162" s="3">
         <v>3</v>
       </c>
-      <c r="M162" s="2">
+      <c r="M162" s="4">
         <v>0.223972385</v>
       </c>
-      <c r="N162" s="2">
+      <c r="N162" s="4">
         <v>0.232663391</v>
       </c>
-      <c r="O162" s="2">
+      <c r="O162" s="4">
         <v>4.028163578</v>
       </c>
-      <c r="P162">
+      <c r="P162" s="3">
         <f t="shared" si="8"/>
         <v>3.8065374886439039E-2</v>
       </c>
-      <c r="Q162">
+      <c r="Q162" s="3">
         <f>ABS(N162-M162)/$T$163</f>
         <v>3.9422239206703812E-2</v>
       </c>

</xml_diff>